<commit_message>
the reports part is working
</commit_message>
<xml_diff>
--- a/server/public/modelsReports.xlsx
+++ b/server/public/modelsReports.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="1333">
   <si>
     <t>Solde N</t>
   </si>
@@ -3332,6 +3332,9 @@
     <t xml:space="preserve">ECARTS DE CONVERSION PASSIF (circulant)                   (H) </t>
   </si>
   <si>
+    <t>TOTAL II (F+G+H)</t>
+  </si>
+  <si>
     <t>EC117</t>
   </si>
   <si>
@@ -3345,6 +3348,9 @@
   </si>
   <si>
     <t>•        Banques (soldes créditeurs)</t>
+  </si>
+  <si>
+    <t>TOTAL GENERAL I + II + III</t>
   </si>
   <si>
     <t>NumEC1</t>
@@ -4884,7 +4890,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5076,7 +5082,7 @@
       <alignment textRotation="255"/>
     </xf>
     <xf borderId="37" fillId="0" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="11" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="28" fillId="0" fontId="11" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -5088,13 +5094,13 @@
     <xf borderId="7" fillId="0" fontId="11" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="34" fillId="0" fontId="11" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="41" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="7" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment textRotation="255"/>
     </xf>
     <xf borderId="8" fillId="7" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="10" fillId="9" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -5114,6 +5120,9 @@
     </xf>
     <xf borderId="7" fillId="0" fontId="22" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="22" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="32" fillId="0" fontId="22" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="43" fillId="0" fontId="22" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -21422,537 +21431,491 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>1080</v>
+      </c>
       <c r="B20" s="53" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D20" s="102">
+        <f>SUM(D21:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="103"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="53" t="s">
         <v>1022</v>
       </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="95"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="53" t="s">
-        <v>973</v>
-      </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="62"/>
+      <c r="C21" s="88" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D21" s="62">
+        <f>SUM('Numéro des comptes V2'!F42)-SUM('Numéro des comptes V2'!E42)</f>
+        <v>0</v>
+      </c>
       <c r="E21" s="95"/>
+      <c r="F21" s="17">
+        <v>141.0</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="B22" s="53" t="s">
-        <v>989</v>
-      </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="62"/>
+        <v>1004</v>
+      </c>
+      <c r="C22" s="88" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D22" s="62">
+        <f>SUM('Numéro des comptes V2'!F44:F51) - SUM('Numéro des comptes V2'!E44:E51)</f>
+        <v>0</v>
+      </c>
       <c r="E22" s="95"/>
+      <c r="F22" s="17">
+        <v>148.0</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="53" t="s">
-        <v>973</v>
-      </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="97"/>
+      <c r="A23" s="8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B23" s="85"/>
+      <c r="C23" s="101" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D23" s="102">
+        <f>SUM(D24:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="103"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B24" s="53" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C24" s="74" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D24" s="102">
-        <f>SUM(D25:D26)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="103"/>
+      <c r="A24" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="104"/>
+      <c r="C24" s="88" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D24" s="62">
+        <f>SUM('Numéro des comptes V2'!F53:F59) - SUM('Numéro des comptes V2'!E53:E59)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="95"/>
+      <c r="F24" s="17">
+        <v>151.0</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>1022</v>
-      </c>
+      <c r="A25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="104"/>
       <c r="C25" s="88" t="s">
-        <v>1082</v>
+        <v>1087</v>
       </c>
       <c r="D25" s="62">
-        <f>SUM('Numéro des comptes V2'!F42)-SUM('Numéro des comptes V2'!E42)</f>
+        <f>SUM('Numéro des comptes V2'!F61:F64) - SUM('Numéro des comptes V2'!E61:E64)</f>
         <v>0</v>
       </c>
       <c r="E25" s="95"/>
       <c r="F25" s="17">
-        <v>141.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C26" s="88" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D26" s="62">
-        <f>SUM('Numéro des comptes V2'!F44:F51) - SUM('Numéro des comptes V2'!E44:E51)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="95"/>
-      <c r="F26" s="17">
-        <v>148.0</v>
-      </c>
+        <v>1088</v>
+      </c>
+      <c r="B26" s="85"/>
+      <c r="C26" s="101" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D26" s="102">
+        <f>SUM(D27:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="103"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="53" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C27" s="88"/>
-      <c r="D27" s="62"/>
+      <c r="A27" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="104"/>
+      <c r="C27" s="88" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D27" s="62">
+        <f>SUM('Numéro des comptes V2'!F69)-SUM('Numéro des comptes V2'!E69)</f>
+        <v>0</v>
+      </c>
       <c r="E27" s="95"/>
+      <c r="F27" s="17">
+        <v>171.0</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="53" t="s">
-        <v>977</v>
-      </c>
-      <c r="C28" s="88"/>
-      <c r="D28" s="62"/>
+      <c r="A28" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="104"/>
+      <c r="C28" s="88" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D28" s="62">
+        <f>SUM('Numéro des comptes V2'!F71)-SUM('Numéro des comptes V2'!E71)</f>
+        <v>0</v>
+      </c>
       <c r="E28" s="95"/>
+      <c r="F28" s="17">
+        <v>172.0</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="53" t="s">
-        <v>994</v>
-      </c>
-      <c r="C29" s="88"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="95"/>
+      <c r="B29" s="105" t="s">
+        <v>958</v>
+      </c>
+      <c r="C29" s="106" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D29" s="107">
+        <f>SUM(D16,D17,D20,D23,D26)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="108"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="85"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="97"/>
+      <c r="A30" s="8" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C30" s="109" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D30" s="102">
+        <f>SUM(D31:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="103"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>1084</v>
-      </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="101" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D31" s="102">
-        <f>SUM(D32:D33)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="103"/>
+        <v>398</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C31" s="88" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D31" s="62">
+        <f>SUM('Numéro des comptes V2'!F328:F334) - SUM('Numéro des comptes V2'!E328:E334)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="95"/>
+      <c r="F31" s="17">
+        <v>441.0</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="104"/>
+      <c r="A32" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>977</v>
+      </c>
       <c r="C32" s="88" t="s">
-        <v>1086</v>
+        <v>1095</v>
       </c>
       <c r="D32" s="62">
-        <f>SUM('Numéro des comptes V2'!F53:F59) - SUM('Numéro des comptes V2'!E53:E59)</f>
+        <f>SUM('Numéro des comptes V2'!F336:F339) - SUM('Numéro des comptes V2'!E336:E339)</f>
         <v>0</v>
       </c>
       <c r="E32" s="95"/>
       <c r="F32" s="17">
-        <v>151.0</v>
+        <v>442.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="104"/>
+      <c r="A33" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>1002</v>
+      </c>
       <c r="C33" s="88" t="s">
-        <v>1087</v>
+        <v>1096</v>
       </c>
       <c r="D33" s="62">
-        <f>SUM('Numéro des comptes V2'!F61:F64) - SUM('Numéro des comptes V2'!E61:E64)</f>
+        <f>SUM('Numéro des comptes V2'!F341:F345) - SUM('Numéro des comptes V2'!E341:E345)</f>
         <v>0</v>
       </c>
       <c r="E33" s="95"/>
       <c r="F33" s="17">
-        <v>155.0</v>
+        <v>443.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B34" s="85"/>
-      <c r="C34" s="101" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D34" s="102">
-        <f>SUM(D35:D36)</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="103"/>
+        <v>420</v>
+      </c>
+      <c r="B34" s="53"/>
+      <c r="C34" s="88" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D34" s="62">
+        <f>SUM('Numéro des comptes V2'!F347:F351) - SUM('Numéro des comptes V2'!E347:E351)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="95"/>
+      <c r="F34" s="17">
+        <v>444.0</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="104"/>
+      <c r="A35" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>994</v>
+      </c>
       <c r="C35" s="88" t="s">
-        <v>1090</v>
+        <v>1098</v>
       </c>
       <c r="D35" s="62">
-        <f>SUM('Numéro des comptes V2'!F69)-SUM('Numéro des comptes V2'!E69)</f>
+        <f>SUM('Numéro des comptes V2'!F353:F361) - SUM('Numéro des comptes V2'!E353:E361)</f>
         <v>0</v>
       </c>
       <c r="E35" s="95"/>
       <c r="F35" s="17">
-        <v>171.0</v>
+        <v>445.0</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="104"/>
+      <c r="A36" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>977</v>
+      </c>
       <c r="C36" s="88" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="D36" s="62">
-        <f>SUM('Numéro des comptes V2'!F71)-SUM('Numéro des comptes V2'!E71)</f>
+        <f>SUM('Numéro des comptes V2'!F363:F368)- SUM('Numéro des comptes V2'!E363:E368)</f>
         <v>0</v>
       </c>
       <c r="E36" s="95"/>
       <c r="F36" s="17">
-        <v>172.0</v>
+        <v>446.0</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="105" t="s">
-        <v>958</v>
-      </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107">
-        <f>SUM(D16,D17,D24,D31,D34)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="108"/>
+      <c r="A37" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="B37" s="53" t="s">
+        <v>975</v>
+      </c>
+      <c r="C37" s="88" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D37" s="62">
+        <f>SUM('Numéro des comptes V2'!F370:F375) - SUM('Numéro des comptes V2'!E370:E375)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="95"/>
+      <c r="F37" s="17">
+        <v>448.0</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>1092</v>
+        <v>453</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C38" s="109" t="s">
-        <v>1093</v>
-      </c>
-      <c r="D38" s="102">
-        <f>SUM(D39:D46)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="103"/>
+        <v>975</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D38" s="64">
+        <f>SUM('Numéro des comptes V2'!F377:F380) - SUM('Numéro des comptes V2'!E377:E380)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="97"/>
+      <c r="F38" s="17">
+        <v>449.0</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>398</v>
+        <v>459</v>
       </c>
       <c r="B39" s="53" t="s">
-        <v>1032</v>
-      </c>
-      <c r="C39" s="88" t="s">
-        <v>1094</v>
-      </c>
-      <c r="D39" s="62">
-        <f>SUM('Numéro des comptes V2'!F328:F334) - SUM('Numéro des comptes V2'!E328:E334)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="95"/>
+        <v>1004</v>
+      </c>
+      <c r="C39" s="110" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D39" s="111">
+        <f>SUM('Numéro des comptes V2'!F382:F387) - SUM('Numéro des comptes V2'!E382:E387)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="112"/>
       <c r="F39" s="17">
-        <v>441.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="B40" s="53" t="s">
-        <v>977</v>
-      </c>
-      <c r="C40" s="88" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D40" s="62">
-        <f>SUM('Numéro des comptes V2'!F336:F339) - SUM('Numéro des comptes V2'!E336:E339)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="95"/>
+      <c r="A40" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B40" s="68" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C40" s="110" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D40" s="111">
+        <f>SUM('Numéro des comptes V2'!F389:F390) - SUM('Numéro des comptes V2'!E389:E390)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="112"/>
       <c r="F40" s="17">
-        <v>442.0</v>
+        <v>470.0</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="B41" s="53" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C41" s="88" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D41" s="62">
-        <f>SUM('Numéro des comptes V2'!F341:F345) - SUM('Numéro des comptes V2'!E341:E345)</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="95"/>
-      <c r="F41" s="17">
-        <v>443.0</v>
-      </c>
+      <c r="B41" s="78"/>
+      <c r="C41" s="106" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D41" s="107">
+        <f>SUM(D30,D39:D40)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="108"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="88" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D42" s="62">
-        <f>SUM('Numéro des comptes V2'!F347:F351) - SUM('Numéro des comptes V2'!E347:E351)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="95"/>
-      <c r="F42" s="17">
-        <v>444.0</v>
-      </c>
+        <v>1105</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>987</v>
+      </c>
+      <c r="C42" s="113" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D42" s="114"/>
+      <c r="E42" s="115"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>427</v>
+        <v>489</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>994</v>
+        <v>975</v>
       </c>
       <c r="C43" s="88" t="s">
-        <v>1098</v>
+        <v>1107</v>
       </c>
       <c r="D43" s="62">
-        <f>SUM('Numéro des comptes V2'!F353:F361) - SUM('Numéro des comptes V2'!E353:E361)</f>
+        <f>SUM('Numéro des comptes V2'!F412)-SUM('Numéro des comptes V2'!E412)</f>
         <v>0</v>
       </c>
       <c r="E43" s="95"/>
       <c r="F43" s="17">
-        <v>445.0</v>
+        <v>552.0</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>438</v>
+        <v>491</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="C44" s="88" t="s">
-        <v>1099</v>
+        <v>1108</v>
       </c>
       <c r="D44" s="62">
-        <f>SUM('Numéro des comptes V2'!F363:F368)- SUM('Numéro des comptes V2'!E363:E368)</f>
+        <f>SUM('Numéro des comptes V2'!F414)-SUM('Numéro des comptes V2'!E414)</f>
         <v>0</v>
       </c>
       <c r="E44" s="95"/>
       <c r="F44" s="17">
-        <v>446.0</v>
+        <v>553.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>445</v>
+        <v>493</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>975</v>
-      </c>
-      <c r="C45" s="88" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D45" s="62">
-        <f>SUM('Numéro des comptes V2'!F370:F375) - SUM('Numéro des comptes V2'!E370:E375)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="95"/>
+        <v>1032</v>
+      </c>
+      <c r="C45" s="96" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D45" s="64">
+        <f>SUM('Numéro des comptes V2'!F416:F417) - SUM('Numéro des comptes V2'!E416:E417)</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="97"/>
       <c r="F45" s="17">
-        <v>448.0</v>
+        <v>554.0</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="B46" s="53" t="s">
-        <v>975</v>
-      </c>
-      <c r="C46" s="96" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D46" s="64">
-        <f>SUM('Numéro des comptes V2'!F377:F380) - SUM('Numéro des comptes V2'!E377:E380)</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="97"/>
-      <c r="F46" s="17">
-        <v>449.0</v>
-      </c>
+      <c r="B46" s="78" t="s">
+        <v>997</v>
+      </c>
+      <c r="C46" s="116" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D46" s="107">
+        <f>SUM(D43:D45)</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="108"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="B47" s="53" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C47" s="110" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D47" s="111">
-        <f>SUM('Numéro des comptes V2'!F382:F387) - SUM('Numéro des comptes V2'!E382:E387)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="112"/>
-      <c r="F47" s="17">
-        <v>450.0</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="14" t="s">
-        <v>463</v>
-      </c>
-      <c r="B48" s="68" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C48" s="110" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D48" s="111">
-        <f>SUM('Numéro des comptes V2'!F389:F390) - SUM('Numéro des comptes V2'!E389:E390)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="112"/>
-      <c r="F48" s="17">
-        <v>470.0</v>
-      </c>
-    </row>
+      <c r="B47" s="117" t="s">
+        <v>958</v>
+      </c>
+      <c r="C47" s="118" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D47" s="55">
+        <f>SUM(D29,D41,D46)</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="56"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="78"/>
-      <c r="C49" s="106"/>
-      <c r="D49" s="107">
-        <f>SUM(D38,D47:D48)</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="108"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="8" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B50" s="53" t="s">
-        <v>987</v>
-      </c>
-      <c r="C50" s="113" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D50" s="114"/>
-      <c r="E50" s="115"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="B51" s="53" t="s">
-        <v>975</v>
-      </c>
-      <c r="C51" s="88" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D51" s="62">
-        <f>SUM('Numéro des comptes V2'!F412)-SUM('Numéro des comptes V2'!E412)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="95"/>
-      <c r="F51" s="17">
-        <v>552.0</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="B52" s="53" t="s">
-        <v>973</v>
-      </c>
-      <c r="C52" s="88" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D52" s="62">
-        <f>SUM('Numéro des comptes V2'!F414)-SUM('Numéro des comptes V2'!E414)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="95"/>
-      <c r="F52" s="17">
-        <v>553.0</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="8" t="s">
-        <v>493</v>
-      </c>
-      <c r="B53" s="53" t="s">
-        <v>1032</v>
-      </c>
-      <c r="C53" s="96" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D53" s="64">
-        <f>SUM('Numéro des comptes V2'!F416:F417) - SUM('Numéro des comptes V2'!E416:E417)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="97"/>
-      <c r="F53" s="17">
-        <v>554.0</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="78" t="s">
-        <v>997</v>
-      </c>
-      <c r="C54" s="116"/>
-      <c r="D54" s="107">
-        <f>SUM(D51:D53)</f>
-        <v>0</v>
-      </c>
-      <c r="E54" s="108"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="117" t="s">
-        <v>958</v>
-      </c>
-      <c r="C55" s="118"/>
-      <c r="D55" s="55">
-        <f>SUM(D37,D49,D54)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="56"/>
-    </row>
+      <c r="E49" s="54"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="E57" s="54"/>
-    </row>
+    <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1"/>
@@ -22885,14 +22848,6 @@
     <row r="987" ht="15.75" customHeight="1"/>
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -22922,36 +22877,36 @@
     <row r="1" ht="14.25" customHeight="1"/>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="D2" s="119" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="E2" s="120" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="F2" s="120" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="G2" s="120" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="H2" s="120" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="E3" s="122"/>
       <c r="F3" s="122"/>
@@ -22966,22 +22921,21 @@
         <v>778</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="D4" s="124" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="E4" s="125">
         <f>SUM('Numéro des comptes V2'!F669:F670,'Numéro des comptes V2'!F672) - SUM('Numéro des comptes V2'!E669:E670,'Numéro des comptes V2'!E672)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="125">
-        <f>SUM('Numéro des comptes V2'!F671) - SUM('Numéro des comptes V2'!E671)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="125">
+      <c r="F4" s="126" t="s">
+        <v>958</v>
+      </c>
+      <c r="G4" s="125" t="str">
         <f t="shared" ref="G4:G10" si="1">E4+F4</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H4" s="125"/>
       <c r="I4" s="8">
@@ -22996,10 +22950,10 @@
         <v>800</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D5" s="126" t="s">
-        <v>1122</v>
+        <v>1123</v>
+      </c>
+      <c r="D5" s="127" t="s">
+        <v>1124</v>
       </c>
       <c r="E5" s="122">
         <f>SUM('Numéro des comptes V2'!F674:F696,'Numéro des comptes V2'!F698:F702) - SUM('Numéro des comptes V2'!E674:E696,'Numéro des comptes V2'!E698:E702)</f>
@@ -23019,8 +22973,8 @@
       <c r="A6" s="8" t="s">
         <v>807</v>
       </c>
-      <c r="D6" s="127" t="s">
-        <v>1123</v>
+      <c r="D6" s="128" t="s">
+        <v>1125</v>
       </c>
       <c r="E6" s="122">
         <f>SUM('Numéro des comptes V2'!F705:F716) - SUM('Numéro des comptes V2'!E705:E716)</f>
@@ -23044,16 +22998,16 @@
         <v>826</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D7" s="128" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E7" s="129">
+        <v>1126</v>
+      </c>
+      <c r="D7" s="129" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E7" s="130">
         <f>SUM('Numéro des comptes V2'!F718:F720) - SUM('Numéro des comptes V2'!E718:E720)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="129">
+      <c r="F7" s="130">
         <f>SUM('Numéro des comptes V2'!F721) - SUM('Numéro des comptes V2'!E721)</f>
         <v>0</v>
       </c>
@@ -23071,10 +23025,10 @@
         <v>831</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D8" s="127" t="s">
-        <v>1127</v>
+        <v>1128</v>
+      </c>
+      <c r="D8" s="128" t="s">
+        <v>1129</v>
       </c>
       <c r="E8" s="122">
         <f>SUM('Numéro des comptes V2'!F723) - SUM('Numéro des comptes V2'!E723)</f>
@@ -23098,16 +23052,16 @@
         <v>838</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D9" s="127" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E9" s="130">
+        <v>1130</v>
+      </c>
+      <c r="D9" s="128" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E9" s="131">
         <f>SUM('Numéro des comptes V2'!F726:F729) - SUM('Numéro des comptes V2'!E726:E729)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="130">
+      <c r="F9" s="131">
         <f>SUM('Numéro des comptes V2'!F730) - SUM('Numéro des comptes V2'!E730)</f>
         <v>0</v>
       </c>
@@ -23125,16 +23079,16 @@
         <v>855</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D10" s="126" t="s">
-        <v>1131</v>
-      </c>
-      <c r="E10" s="131">
+        <v>1132</v>
+      </c>
+      <c r="D10" s="127" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E10" s="132">
         <f>SUM('Numéro des comptes V2'!F732:F744) - SUM('Numéro des comptes V2'!E732:E744)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="130">
+      <c r="F10" s="131">
         <f>SUM('Numéro des comptes V2'!F746:F747) - SUM('Numéro des comptes V2'!E746:E747)</f>
         <v>0</v>
       </c>
@@ -23145,29 +23099,29 @@
       <c r="H10" s="125"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="D11" s="132" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E11" s="133">
+      <c r="D11" s="133" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E11" s="134">
         <f t="shared" ref="E11:G11" si="2">SUM(E4:E10)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="133" t="str">
+      <c r="F11" s="134" t="str">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="G11" s="125" t="str">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H11" s="133"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" s="134"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="D12" s="121" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="E12" s="125"/>
       <c r="F12" s="125"/>
@@ -23182,10 +23136,10 @@
         <v>503</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D13" s="134" t="s">
-        <v>1136</v>
+        <v>1137</v>
+      </c>
+      <c r="D13" s="135" t="s">
+        <v>1138</v>
       </c>
       <c r="E13" s="125">
         <f>SUM('Numéro des comptes V2'!E421:E423,'Numéro des comptes V2'!E425) - SUM('Numéro des comptes V2'!F421:F423,'Numéro des comptes V2'!F425)</f>
@@ -23209,10 +23163,10 @@
         <v>535</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D14" s="126" t="s">
-        <v>1138</v>
+        <v>1139</v>
+      </c>
+      <c r="D14" s="127" t="s">
+        <v>1140</v>
       </c>
       <c r="E14" s="125">
         <f>SUM('Numéro des comptes V2'!E427:E454,'Numéro des comptes V2'!E456:E461) - SUM('Numéro des comptes V2'!F427:F454,'Numéro des comptes V2'!F456:F461)</f>
@@ -23236,16 +23190,16 @@
         <v>612</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D15" s="127" t="s">
-        <v>1140</v>
+        <v>1141</v>
+      </c>
+      <c r="D15" s="128" t="s">
+        <v>1142</v>
       </c>
       <c r="E15" s="122">
         <f>SUM('Numéro des comptes V2'!E464:E528,'Numéro des comptes V2'!E530) - SUM('Numéro des comptes V2'!F464:F528,'Numéro des comptes V2'!F530)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="135">
+      <c r="F15" s="136">
         <f>SUM('Numéro des comptes V2'!E529) - SUM('Numéro des comptes V2'!F529)</f>
         <v>0</v>
       </c>
@@ -23263,12 +23217,12 @@
         <v>626</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D16" s="127" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E16" s="130">
+        <v>1143</v>
+      </c>
+      <c r="D16" s="128" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E16" s="131">
         <f>SUM('Numéro des comptes V2'!E532:E541) - SUM('Numéro des comptes V2'!F532:F541)</f>
         <v>0</v>
       </c>
@@ -23276,7 +23230,7 @@
         <f>SUM('Numéro des comptes V2'!E529) - SUM('Numéro des comptes V2'!F529)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="136">
+      <c r="G16" s="137">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23290,10 +23244,10 @@
         <v>652</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D17" s="127" t="s">
-        <v>1144</v>
+        <v>1145</v>
+      </c>
+      <c r="D17" s="128" t="s">
+        <v>1146</v>
       </c>
       <c r="E17" s="122">
         <f>SUM('Numéro des comptes V2'!E543:E565) - SUM('Numéro des comptes V2'!F543:F565)</f>
@@ -23317,12 +23271,12 @@
         <v>660</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D18" s="127" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E18" s="130">
+        <v>1147</v>
+      </c>
+      <c r="D18" s="128" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E18" s="131">
         <f>SUM('Numéro des comptes V2'!E568:E571) - SUM('Numéro des comptes V2'!F568:F571)</f>
         <v>0</v>
       </c>
@@ -23344,16 +23298,16 @@
         <v>688</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D19" s="128" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E19" s="137">
+        <v>1149</v>
+      </c>
+      <c r="D19" s="129" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E19" s="138">
         <f>SUM('Numéro des comptes V2'!E574:E597) - SUM('Numéro des comptes V2'!F574:F597)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="130">
+      <c r="F19" s="131">
         <f>SUM('Numéro des comptes V2'!E599:E600) - SUM('Numéro des comptes V2'!F599:F600)</f>
         <v>0</v>
       </c>
@@ -23361,17 +23315,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H19" s="138"/>
+      <c r="H19" s="139"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="D20" s="139" t="s">
-        <v>1149</v>
-      </c>
-      <c r="E20" s="140">
+      <c r="D20" s="140" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E20" s="141">
         <f t="shared" ref="E20:G20" si="4">SUM(E13:E19)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="141" t="str">
+      <c r="F20" s="142" t="str">
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
@@ -23379,20 +23333,20 @@
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
-      <c r="H20" s="142"/>
+      <c r="H20" s="143"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>1150</v>
-      </c>
-      <c r="D21" s="143" t="s">
-        <v>1151</v>
-      </c>
-      <c r="E21" s="144">
+        <v>1152</v>
+      </c>
+      <c r="D21" s="144" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E21" s="145">
         <f t="shared" ref="E21:F21" si="5">E11-E20</f>
         <v>0</v>
       </c>
-      <c r="F21" s="144" t="str">
+      <c r="F21" s="145" t="str">
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
@@ -23400,19 +23354,19 @@
         <f>E21+F21</f>
         <v>#REF!</v>
       </c>
-      <c r="H21" s="145"/>
+      <c r="H21" s="146"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D22" s="121" t="s">
-        <v>1153</v>
-      </c>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
+        <v>1155</v>
+      </c>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
       <c r="G22" s="125"/>
-      <c r="H22" s="147"/>
+      <c r="H22" s="148"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="8" t="s">
@@ -23422,16 +23376,16 @@
         <v>863</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1154</v>
-      </c>
-      <c r="D23" s="148" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E23" s="138">
+        <v>1156</v>
+      </c>
+      <c r="D23" s="149" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E23" s="139">
         <f>SUM('Numéro des comptes V2'!F749:F750) - SUM('Numéro des comptes V2'!E749:E750)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="138">
+      <c r="F23" s="139">
         <f>SUM('Numéro des comptes V2'!F751) - SUM('Numéro des comptes V2'!E751)</f>
         <v>0</v>
       </c>
@@ -23449,16 +23403,16 @@
         <v>868</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D24" s="127" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E24" s="130">
+        <v>1158</v>
+      </c>
+      <c r="D24" s="128" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E24" s="131">
         <f>SUM('Numéro des comptes V2'!F753) - SUM('Numéro des comptes V2'!E753)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="130">
+      <c r="F24" s="131">
         <f>SUM('Numéro des comptes V2'!F754) - SUM('Numéro des comptes V2'!E754)</f>
         <v>0</v>
       </c>
@@ -23476,12 +23430,12 @@
         <v>879</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1158</v>
-      </c>
-      <c r="D25" s="127" t="s">
-        <v>1159</v>
-      </c>
-      <c r="E25" s="130">
+        <v>1160</v>
+      </c>
+      <c r="D25" s="128" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E25" s="131">
         <f>SUM('Numéro des comptes V2'!F756:F762) - SUM('Numéro des comptes V2'!E756:E762)</f>
         <v>0</v>
       </c>
@@ -23503,16 +23457,16 @@
         <v>892</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1160</v>
-      </c>
-      <c r="D26" s="149" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E26" s="130">
+        <v>1162</v>
+      </c>
+      <c r="D26" s="150" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E26" s="131">
         <f>SUM('Numéro des comptes V2'!F765:F773) - SUM('Numéro des comptes V2'!E765:E773)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="130">
+      <c r="F26" s="131">
         <f>SUM('Numéro des comptes V2'!F774) - SUM('Numéro des comptes V2'!E774)</f>
         <v>0</v>
       </c>
@@ -23523,14 +23477,14 @@
       <c r="H26" s="125"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="D27" s="132" t="s">
-        <v>1162</v>
-      </c>
-      <c r="E27" s="150">
+      <c r="D27" s="133" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E27" s="151">
         <f t="shared" ref="E27:G27" si="7">SUM(E23:E26)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="150">
+      <c r="F27" s="151">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -23538,19 +23492,19 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H27" s="150"/>
+      <c r="H27" s="151"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="D28" s="121" t="s">
-        <v>1164</v>
-      </c>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
+        <v>1166</v>
+      </c>
+      <c r="E28" s="147"/>
+      <c r="F28" s="147"/>
       <c r="G28" s="125"/>
-      <c r="H28" s="151"/>
+      <c r="H28" s="152"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="8" t="s">
@@ -23560,12 +23514,12 @@
         <v>700</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D29" s="148" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E29" s="152">
+        <v>1167</v>
+      </c>
+      <c r="D29" s="149" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E29" s="153">
         <f>SUM('Numéro des comptes V2'!E602:E607) - SUM('Numéro des comptes V2'!F602:F607)</f>
         <v>0</v>
       </c>
@@ -23587,16 +23541,16 @@
         <v>705</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D30" s="127" t="s">
-        <v>1168</v>
-      </c>
-      <c r="E30" s="130">
+        <v>1169</v>
+      </c>
+      <c r="D30" s="128" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E30" s="131">
         <f>SUM('Numéro des comptes V2'!E610) - SUM('Numéro des comptes V2'!F610)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="130">
+      <c r="F30" s="131">
         <f>SUM('Numéro des comptes V2'!E611) - SUM('Numéro des comptes V2'!F611)</f>
         <v>0</v>
       </c>
@@ -23614,10 +23568,10 @@
         <v>712</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1169</v>
-      </c>
-      <c r="D31" s="127" t="s">
-        <v>1170</v>
+        <v>1171</v>
+      </c>
+      <c r="D31" s="128" t="s">
+        <v>1172</v>
       </c>
       <c r="E31" s="122">
         <f>SUM('Numéro des comptes V2'!E613:E615) - SUM('Numéro des comptes V2'!F613:F615)</f>
@@ -23641,12 +23595,12 @@
         <v>721</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D32" s="127" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E32" s="130">
+        <v>1173</v>
+      </c>
+      <c r="D32" s="128" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E32" s="131">
         <f>SUM('Numéro des comptes V2'!E618:E622) - SUM('Numéro des comptes V2'!F618:F622)</f>
         <v>0</v>
       </c>
@@ -23661,78 +23615,78 @@
       <c r="H32" s="125"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="D33" s="132" t="s">
-        <v>1173</v>
-      </c>
-      <c r="E33" s="133">
+      <c r="D33" s="133" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E33" s="134">
         <f t="shared" ref="E33:G33" si="9">SUM(E29:E32)</f>
         <v>0</v>
       </c>
-      <c r="F33" s="133">
+      <c r="F33" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G33" s="133">
+      <c r="G33" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H33" s="133"/>
+      <c r="H33" s="134"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D34" s="153" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E34" s="144">
+        <v>1176</v>
+      </c>
+      <c r="D34" s="154" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E34" s="145">
         <f t="shared" ref="E34:G34" si="10">E27-E33</f>
         <v>0</v>
       </c>
-      <c r="F34" s="144">
+      <c r="F34" s="145">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G34" s="150">
+      <c r="G34" s="151">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H34" s="150"/>
+      <c r="H34" s="151"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
-      <c r="D35" s="153" t="s">
-        <v>1177</v>
-      </c>
-      <c r="E35" s="154">
+      <c r="D35" s="154" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E35" s="155">
         <f>E34+E21</f>
         <v>0</v>
       </c>
-      <c r="F35" s="154" t="str">
+      <c r="F35" s="155" t="str">
         <f>F21+F34</f>
         <v>#REF!</v>
       </c>
-      <c r="G35" s="150" t="str">
+      <c r="G35" s="151" t="str">
         <f>E35+F35</f>
         <v>#REF!</v>
       </c>
-      <c r="H35" s="145"/>
+      <c r="H35" s="146"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="D36" s="121" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="E36" s="122"/>
-      <c r="F36" s="151"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="151"/>
+      <c r="F36" s="152"/>
+      <c r="G36" s="151"/>
+      <c r="H36" s="152"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="8" t="s">
@@ -23742,10 +23696,10 @@
         <v>899</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1180</v>
-      </c>
-      <c r="D37" s="155" t="s">
-        <v>1181</v>
+        <v>1182</v>
+      </c>
+      <c r="D37" s="156" t="s">
+        <v>1183</v>
       </c>
       <c r="E37" s="125">
         <f>SUM('Numéro des comptes V2'!F776:F778) - SUM('Numéro des comptes V2'!E776:E778)</f>
@@ -23769,10 +23723,10 @@
         <v>904</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D38" s="156" t="s">
-        <v>1183</v>
+        <v>1184</v>
+      </c>
+      <c r="D38" s="157" t="s">
+        <v>1185</v>
       </c>
       <c r="E38" s="122">
         <f>SUM('Numéro des comptes V2'!F781) - SUM('Numéro des comptes V2'!E781)</f>
@@ -23796,12 +23750,12 @@
         <v>909</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1184</v>
-      </c>
-      <c r="D39" s="155" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E39" s="130">
+        <v>1186</v>
+      </c>
+      <c r="D39" s="156" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E39" s="131">
         <f>SUM('Numéro des comptes V2'!F784) - SUM('Numéro des comptes V2'!E784)</f>
         <v>0</v>
       </c>
@@ -23823,16 +23777,16 @@
         <v>919</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1186</v>
-      </c>
-      <c r="D40" s="156" t="s">
-        <v>1187</v>
+        <v>1188</v>
+      </c>
+      <c r="D40" s="157" t="s">
+        <v>1189</v>
       </c>
       <c r="E40" s="122">
         <f>SUM('Numéro des comptes V2'!F787:F795) - SUM('Numéro des comptes V2'!E787:E795)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="130">
+      <c r="F40" s="131">
         <f>SUM('Numéro des comptes V2'!F796) - SUM('Numéro des comptes V2'!E796)</f>
         <v>0</v>
       </c>
@@ -23850,16 +23804,16 @@
         <v>940</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D41" s="157" t="s">
-        <v>1189</v>
-      </c>
-      <c r="E41" s="130">
+        <v>1190</v>
+      </c>
+      <c r="D41" s="158" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E41" s="131">
         <f>SUM('Numéro des comptes V2'!F798:F814) - SUM('Numéro des comptes V2'!E798:E814)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="129">
+      <c r="F41" s="130">
         <f>SUM('Numéro des comptes V2'!F815) - SUM('Numéro des comptes V2'!E815)</f>
         <v>0</v>
       </c>
@@ -23870,14 +23824,14 @@
       <c r="H41" s="125"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="D42" s="158" t="s">
-        <v>1190</v>
-      </c>
-      <c r="E42" s="150">
+      <c r="D42" s="159" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E42" s="151">
         <f t="shared" ref="E42:F42" si="12">SUM(E37:E41)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="150">
+      <c r="F42" s="151">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -23885,19 +23839,19 @@
         <f>SUM(G37:G42)</f>
         <v>#REF!</v>
       </c>
-      <c r="H42" s="150"/>
+      <c r="H42" s="151"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="D43" s="121" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="159"/>
+        <v>1194</v>
+      </c>
+      <c r="E43" s="147"/>
+      <c r="F43" s="147"/>
+      <c r="G43" s="160"/>
+      <c r="H43" s="160"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="8" t="s">
@@ -23907,10 +23861,10 @@
         <v>728</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1193</v>
-      </c>
-      <c r="D44" s="126" t="s">
-        <v>1194</v>
+        <v>1195</v>
+      </c>
+      <c r="D44" s="127" t="s">
+        <v>1196</v>
       </c>
       <c r="E44" s="125">
         <f>SUM('Numéro des comptes V2'!E625:E627) - SUM('Numéro des comptes V2'!F625:F627)</f>
@@ -23934,16 +23888,16 @@
         <v>733</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D45" s="148" t="s">
-        <v>1196</v>
+        <v>1197</v>
+      </c>
+      <c r="D45" s="149" t="s">
+        <v>1198</v>
       </c>
       <c r="E45" s="125">
         <f>SUM('Numéro des comptes V2'!E630) - SUM('Numéro des comptes V2'!F630)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="160">
+      <c r="F45" s="161">
         <f>SUM('Numéro des comptes V2'!E631) - SUM('Numéro des comptes V2'!F631)</f>
         <v>0</v>
       </c>
@@ -23961,16 +23915,16 @@
         <v>747</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D46" s="161" t="s">
-        <v>1198</v>
-      </c>
-      <c r="E46" s="131">
+        <v>1199</v>
+      </c>
+      <c r="D46" s="162" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E46" s="132">
         <f>SUM('Numéro des comptes V2'!E633:E644) - SUM('Numéro des comptes V2'!F633:F644)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="130">
+      <c r="F46" s="131">
         <f>SUM('Numéro des comptes V2'!E645) - SUM('Numéro des comptes V2'!F645)</f>
         <v>0</v>
       </c>
@@ -23988,16 +23942,16 @@
         <v>767</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D47" s="148" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E47" s="130">
+        <v>1201</v>
+      </c>
+      <c r="D47" s="149" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E47" s="131">
         <f>SUM('Numéro des comptes V2'!E648:E650,'Numéro des comptes V2'!E652:E656,'Numéro des comptes V2'!E658:E659,'Numéro des comptes V2'!E661:E662) - SUM('Numéro des comptes V2'!F648:F650,'Numéro des comptes V2'!F652:F656,'Numéro des comptes V2'!F658:F659,'Numéro des comptes V2'!F661:F662)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="138">
+      <c r="F47" s="139">
         <f>SUM('Numéro des comptes V2'!E663) - SUM('Numéro des comptes V2'!F663)</f>
         <v>0</v>
       </c>
@@ -24008,14 +23962,14 @@
       <c r="H47" s="125"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="D48" s="162" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E48" s="140">
+      <c r="D48" s="163" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E48" s="141">
         <f t="shared" ref="E48:F48" si="14">SUM(E44:E47)</f>
         <v>0</v>
       </c>
-      <c r="F48" s="140">
+      <c r="F48" s="141">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -24023,126 +23977,126 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H48" s="140"/>
+      <c r="H48" s="141"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D49" s="163" t="s">
-        <v>1203</v>
-      </c>
-      <c r="E49" s="154">
+        <v>1204</v>
+      </c>
+      <c r="D49" s="164" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E49" s="155">
         <f t="shared" ref="E49:F49" si="15">E42-E48</f>
         <v>0</v>
       </c>
-      <c r="F49" s="144">
+      <c r="F49" s="145">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G49" s="164">
+      <c r="G49" s="165">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H49" s="164"/>
+      <c r="H49" s="165"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="163" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E50" s="165">
+      <c r="D50" s="164" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E50" s="166">
         <f t="shared" ref="E50:F50" si="16">E35+E49</f>
         <v>0</v>
       </c>
-      <c r="F50" s="166" t="str">
+      <c r="F50" s="167" t="str">
         <f t="shared" si="16"/>
         <v>#REF!</v>
       </c>
-      <c r="G50" s="164" t="str">
+      <c r="G50" s="165" t="str">
         <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
-      <c r="H50" s="164"/>
+      <c r="H50" s="165"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="D51" s="167" t="s">
-        <v>1206</v>
-      </c>
-      <c r="E51" s="168">
+      <c r="D51" s="168" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E51" s="169">
         <f>SUM('Numéro des comptes V2'!E665:E667) - SUM('Numéro des comptes V2'!F665:F667)</f>
         <v>0</v>
       </c>
-      <c r="F51" s="169"/>
-      <c r="G51" s="164">
+      <c r="F51" s="170"/>
+      <c r="G51" s="165">
         <f>E51</f>
         <v>0</v>
       </c>
-      <c r="H51" s="164"/>
+      <c r="H51" s="165"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="167" t="s">
-        <v>1207</v>
-      </c>
-      <c r="E52" s="170">
+      <c r="D52" s="168" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E52" s="171">
         <f t="shared" ref="E52:G52" si="17">E50-E51</f>
         <v>0</v>
       </c>
-      <c r="F52" s="170" t="str">
+      <c r="F52" s="171" t="str">
         <f t="shared" si="17"/>
         <v>#REF!</v>
       </c>
-      <c r="G52" s="164" t="str">
+      <c r="G52" s="165" t="str">
         <f t="shared" si="17"/>
         <v>#REF!</v>
       </c>
-      <c r="H52" s="164"/>
+      <c r="H52" s="165"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="D53" s="171" t="s">
-        <v>1208</v>
-      </c>
-      <c r="E53" s="172"/>
-      <c r="F53" s="172"/>
-      <c r="G53" s="145" t="str">
+      <c r="D53" s="172" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E53" s="173"/>
+      <c r="F53" s="173"/>
+      <c r="G53" s="146" t="str">
         <f>SUM(G11,G27,G42)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H53" s="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H53" s="146"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="D54" s="173" t="s">
-        <v>1209</v>
-      </c>
-      <c r="E54" s="172"/>
-      <c r="F54" s="172"/>
-      <c r="G54" s="145" t="str">
+      <c r="D54" s="174" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E54" s="173"/>
+      <c r="F54" s="173"/>
+      <c r="G54" s="146" t="str">
         <f>SUM(G20,G33,G48)</f>
         <v>#REF!</v>
       </c>
-      <c r="H54" s="145"/>
+      <c r="H54" s="146"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="D55" s="174" t="s">
-        <v>1210</v>
-      </c>
-      <c r="E55" s="172"/>
-      <c r="F55" s="172"/>
-      <c r="G55" s="145" t="str">
+      <c r="D55" s="175" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E55" s="173"/>
+      <c r="F55" s="173"/>
+      <c r="G55" s="146" t="str">
         <f>G53-G54</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H55" s="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H55" s="146"/>
     </row>
     <row r="56" ht="14.25" customHeight="1"/>
     <row r="57" ht="14.25" customHeight="1"/>
@@ -25117,581 +25071,581 @@
     <row r="2" ht="14.25" customHeight="1"/>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="175" t="s">
+      <c r="A4" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="176" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C4" s="177" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="179" t="s">
+      <c r="B4" s="177" t="s">
         <v>1213</v>
       </c>
+      <c r="C4" s="178" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D4" s="179"/>
+      <c r="E4" s="180" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="180" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C5" s="181"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="182"/>
+      <c r="B5" s="181" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="183"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>774</v>
       </c>
-      <c r="B6" s="183" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C6" s="184">
+      <c r="B6" s="184" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C6" s="185">
         <f>CPC!E4</f>
         <v>0</v>
       </c>
-      <c r="D6" s="185"/>
-      <c r="E6" s="184"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="185"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="B7" s="183" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C7" s="186">
+      <c r="B7" s="184" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C7" s="187">
         <f>CPC!E13</f>
         <v>0</v>
       </c>
-      <c r="D7" s="185"/>
-      <c r="E7" s="186"/>
+      <c r="D7" s="186"/>
+      <c r="E7" s="187"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B8" s="187" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C8" s="188">
+        <v>1219</v>
+      </c>
+      <c r="B8" s="188" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C8" s="189">
         <f>C6-C7</f>
         <v>0</v>
       </c>
-      <c r="D8" s="189"/>
-      <c r="E8" s="188"/>
+      <c r="D8" s="190"/>
+      <c r="E8" s="189"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B9" s="187" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C9" s="189">
+        <v>1221</v>
+      </c>
+      <c r="B9" s="188" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C9" s="190">
         <f>SUM(C10:C12)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="190"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>781</v>
       </c>
-      <c r="B10" s="183" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C10" s="190">
+      <c r="B10" s="184" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C10" s="191">
         <f>CPC!E5</f>
         <v>0</v>
       </c>
-      <c r="D10" s="185"/>
-      <c r="E10" s="190"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="191"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>807</v>
       </c>
-      <c r="B11" s="183" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C11" s="190">
+      <c r="B11" s="184" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C11" s="191">
         <f>CPC!E6</f>
         <v>0</v>
       </c>
-      <c r="D11" s="185"/>
-      <c r="E11" s="190"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="191"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>821</v>
       </c>
-      <c r="B12" s="183" t="s">
-        <v>1223</v>
-      </c>
-      <c r="C12" s="191">
+      <c r="B12" s="184" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C12" s="192">
         <f>CPC!E7</f>
         <v>0</v>
       </c>
-      <c r="D12" s="185"/>
-      <c r="E12" s="191"/>
+      <c r="D12" s="186"/>
+      <c r="E12" s="192"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B13" s="187" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C13" s="192">
+        <v>1226</v>
+      </c>
+      <c r="B13" s="188" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C13" s="193">
         <f>SUM(C14:C15)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="185"/>
-      <c r="E13" s="192"/>
+      <c r="D13" s="186"/>
+      <c r="E13" s="193"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="B14" s="183" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C14" s="190">
+      <c r="B14" s="184" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C14" s="191">
         <f>CPC!E14</f>
         <v>0</v>
       </c>
-      <c r="D14" s="185"/>
-      <c r="E14" s="190"/>
+      <c r="D14" s="186"/>
+      <c r="E14" s="191"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B15" s="183" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C15" s="193">
+      <c r="B15" s="184" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C15" s="194">
         <f>CPC!E15</f>
         <v>0</v>
       </c>
-      <c r="D15" s="185"/>
-      <c r="E15" s="193"/>
+      <c r="D15" s="186"/>
+      <c r="E15" s="194"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B16" s="187" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C16" s="194">
+        <v>1230</v>
+      </c>
+      <c r="B16" s="188" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C16" s="195">
         <f>C8+C9-C13</f>
         <v>0</v>
       </c>
-      <c r="D16" s="185"/>
-      <c r="E16" s="194"/>
+      <c r="D16" s="186"/>
+      <c r="E16" s="195"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>828</v>
       </c>
-      <c r="B17" s="183" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C17" s="190">
+      <c r="B17" s="184" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C17" s="191">
         <f>CPC!E8</f>
         <v>0</v>
       </c>
-      <c r="D17" s="185"/>
-      <c r="E17" s="190"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="191"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="B18" s="183" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C18" s="190">
+      <c r="B18" s="184" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C18" s="191">
         <f>CPC!E16</f>
         <v>0</v>
       </c>
-      <c r="D18" s="185"/>
-      <c r="E18" s="190"/>
+      <c r="D18" s="186"/>
+      <c r="E18" s="191"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="B19" s="183" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C19" s="190">
+      <c r="B19" s="184" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C19" s="191">
         <f>CPC!E17</f>
         <v>0</v>
       </c>
-      <c r="D19" s="185"/>
-      <c r="E19" s="190"/>
+      <c r="D19" s="186"/>
+      <c r="E19" s="191"/>
     </row>
     <row r="20" ht="24.0" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B20" s="195" t="s">
-        <v>1234</v>
-      </c>
-      <c r="C20" s="192">
+        <v>1235</v>
+      </c>
+      <c r="B20" s="196" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C20" s="193">
         <f>C16+C17-C18-C19</f>
         <v>0</v>
       </c>
-      <c r="D20" s="185"/>
-      <c r="E20" s="192"/>
+      <c r="D20" s="186"/>
+      <c r="E20" s="193"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>833</v>
       </c>
-      <c r="B21" s="183" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C21" s="191">
+      <c r="B21" s="184" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C21" s="192">
         <f>CPC!E9</f>
         <v>0</v>
       </c>
-      <c r="D21" s="185"/>
-      <c r="E21" s="191"/>
+      <c r="D21" s="186"/>
+      <c r="E21" s="192"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="B22" s="183" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C22" s="190">
+      <c r="B22" s="184" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C22" s="191">
         <f>CPC!E18</f>
         <v>0</v>
       </c>
-      <c r="D22" s="185"/>
-      <c r="E22" s="190"/>
+      <c r="D22" s="186"/>
+      <c r="E22" s="191"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>840</v>
       </c>
-      <c r="B23" s="183" t="s">
-        <v>1237</v>
-      </c>
-      <c r="C23" s="190">
+      <c r="B23" s="184" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C23" s="191">
         <f>CPC!E26</f>
         <v>0</v>
       </c>
-      <c r="D23" s="185"/>
-      <c r="E23" s="190"/>
+      <c r="D23" s="186"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>662</v>
       </c>
-      <c r="B24" s="183" t="s">
-        <v>1238</v>
-      </c>
-      <c r="C24" s="190">
+      <c r="B24" s="184" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C24" s="191">
         <f>CPC!E19</f>
         <v>0</v>
       </c>
-      <c r="D24" s="185"/>
-      <c r="E24" s="190"/>
+      <c r="D24" s="186"/>
+      <c r="E24" s="191"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B25" s="196" t="s">
-        <v>1239</v>
-      </c>
-      <c r="C25" s="197">
+        <v>1152</v>
+      </c>
+      <c r="B25" s="197" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C25" s="198">
         <f>C20+C21-C22+C23-C24</f>
         <v>0</v>
       </c>
-      <c r="D25" s="192"/>
-      <c r="E25" s="197"/>
+      <c r="D25" s="193"/>
+      <c r="E25" s="198"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>1174</v>
-      </c>
-      <c r="B26" s="196" t="s">
-        <v>1240</v>
-      </c>
-      <c r="C26" s="197">
+        <v>1176</v>
+      </c>
+      <c r="B26" s="197" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C26" s="198">
         <f>CPC!E34</f>
         <v>0</v>
       </c>
-      <c r="D26" s="192"/>
-      <c r="E26" s="197"/>
+      <c r="D26" s="193"/>
+      <c r="E26" s="198"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B27" s="196" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C27" s="197">
+        <v>1178</v>
+      </c>
+      <c r="B27" s="197" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C27" s="198">
         <f>C25+C26</f>
         <v>0</v>
       </c>
-      <c r="D27" s="192"/>
-      <c r="E27" s="197"/>
+      <c r="D27" s="193"/>
+      <c r="E27" s="198"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B28" s="196" t="s">
-        <v>1242</v>
-      </c>
-      <c r="C28" s="197">
+        <v>1204</v>
+      </c>
+      <c r="B28" s="197" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C28" s="198">
         <f>CPC!E49</f>
         <v>0</v>
       </c>
-      <c r="D28" s="192"/>
-      <c r="E28" s="197"/>
+      <c r="D28" s="193"/>
+      <c r="E28" s="198"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="B29" s="183" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C29" s="197">
+      <c r="B29" s="184" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C29" s="198">
         <f>CPC!E51</f>
         <v>0</v>
       </c>
-      <c r="D29" s="185"/>
-      <c r="E29" s="197"/>
+      <c r="D29" s="186"/>
+      <c r="E29" s="198"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="196" t="s">
-        <v>1244</v>
-      </c>
-      <c r="C30" s="197">
+      <c r="B30" s="197" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C30" s="198">
         <f>C27+C28-C29</f>
         <v>0</v>
       </c>
-      <c r="D30" s="192"/>
-      <c r="E30" s="197"/>
+      <c r="D30" s="193"/>
+      <c r="E30" s="198"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="198" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="182"/>
+      <c r="B31" s="199" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C31" s="182"/>
+      <c r="D31" s="182"/>
+      <c r="E31" s="183"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="199" t="s">
-        <v>1246</v>
-      </c>
-      <c r="C32" s="190"/>
-      <c r="D32" s="190"/>
-      <c r="E32" s="190"/>
+      <c r="B32" s="200" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C32" s="191"/>
+      <c r="D32" s="191"/>
+      <c r="E32" s="191"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="200" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C33" s="190">
+      <c r="B33" s="201" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C33" s="191">
         <f>IF(C30&gt;=0,C30,0)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="184"/>
-      <c r="E33" s="190"/>
+      <c r="D33" s="185"/>
+      <c r="E33" s="191"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="B34" s="200" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C34" s="184">
+      <c r="B34" s="201" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C34" s="185">
         <f>IF(C30&lt;0,C30,0)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="184"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="185"/>
+      <c r="E34" s="185"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="8" t="s">
         <v>662</v>
       </c>
-      <c r="B35" s="200" t="s">
-        <v>1249</v>
-      </c>
-      <c r="C35" s="201">
+      <c r="B35" s="201" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C35" s="202">
         <f>CPC!E19</f>
         <v>0</v>
       </c>
-      <c r="D35" s="184"/>
-      <c r="E35" s="191"/>
+      <c r="D35" s="185"/>
+      <c r="E35" s="192"/>
       <c r="F35" s="8" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="B36" s="200" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C36" s="202">
+      <c r="B36" s="201" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C36" s="203">
         <f>CPC!E32</f>
         <v>0</v>
       </c>
-      <c r="D36" s="184"/>
-      <c r="E36" s="190"/>
+      <c r="D36" s="185"/>
+      <c r="E36" s="191"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="B37" s="200" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C37" s="202">
+      <c r="B37" s="201" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C37" s="203">
         <f>CPC!E47</f>
         <v>0</v>
       </c>
-      <c r="D37" s="184"/>
-      <c r="E37" s="190"/>
+      <c r="D37" s="185"/>
+      <c r="E37" s="191"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="8" t="s">
         <v>840</v>
       </c>
-      <c r="B38" s="200" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C38" s="184">
+      <c r="B38" s="201" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C38" s="185">
         <f>CPC!E10</f>
         <v>0</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="190"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="191"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="8" t="s">
         <v>881</v>
       </c>
-      <c r="B39" s="200" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C39" s="184">
+      <c r="B39" s="201" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C39" s="185">
         <f>CPC!E26</f>
         <v>0</v>
       </c>
-      <c r="D39" s="184"/>
-      <c r="E39" s="190"/>
+      <c r="D39" s="185"/>
+      <c r="E39" s="191"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>921</v>
       </c>
-      <c r="B40" s="200" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C40" s="184">
+      <c r="B40" s="201" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C40" s="185">
         <f>CPC!E41</f>
         <v>0</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="190"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="191"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>894</v>
       </c>
-      <c r="B41" s="183" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C41" s="184">
+      <c r="B41" s="184" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C41" s="185">
         <f>CPC!E37</f>
         <v>0</v>
       </c>
-      <c r="D41" s="184"/>
-      <c r="E41" s="190"/>
+      <c r="D41" s="185"/>
+      <c r="E41" s="191"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>723</v>
       </c>
-      <c r="B42" s="183" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C42" s="203">
+      <c r="B42" s="184" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C42" s="204">
         <f>CPC!E44</f>
         <v>0</v>
       </c>
-      <c r="D42" s="184"/>
-      <c r="E42" s="190"/>
+      <c r="D42" s="185"/>
+      <c r="E42" s="191"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B43" s="204" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C43" s="188">
+        <v>1260</v>
+      </c>
+      <c r="B43" s="205" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C43" s="189">
         <f>C32+C33-C34+C35+C36+C37-C38-C39-C40-C41+C42</f>
         <v>0</v>
       </c>
-      <c r="D43" s="194"/>
-      <c r="E43" s="194"/>
+      <c r="D43" s="195"/>
+      <c r="E43" s="195"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B44" s="199" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C44" s="205">
+        <v>1262</v>
+      </c>
+      <c r="B44" s="200" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C44" s="206">
         <f>SUM('Numéro des comptes V2'!F367) - SUM('Numéro des comptes V2'!E367)</f>
         <v>0</v>
       </c>
-      <c r="D44" s="190"/>
-      <c r="E44" s="190"/>
+      <c r="D44" s="191"/>
+      <c r="E44" s="191"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="206" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B45" s="187" t="s">
-        <v>1263</v>
-      </c>
-      <c r="C45" s="207">
+      <c r="A45" s="207" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B45" s="188" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C45" s="208">
         <f>C43-C44</f>
         <v>0</v>
       </c>
-      <c r="D45" s="197"/>
-      <c r="E45" s="197"/>
+      <c r="D45" s="198"/>
+      <c r="E45" s="198"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="B46" s="208"/>
-      <c r="C46" s="186"/>
-      <c r="D46" s="185"/>
-      <c r="E46" s="186"/>
+      <c r="B46" s="209"/>
+      <c r="C46" s="187"/>
+      <c r="D46" s="186"/>
+      <c r="E46" s="187"/>
     </row>
     <row r="47" ht="14.25" customHeight="1"/>
     <row r="48" ht="14.25" customHeight="1"/>
@@ -26678,20 +26632,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="209" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B1" s="210" t="s">
-        <v>1265</v>
-      </c>
-      <c r="C1" s="210" t="s">
+      <c r="A1" s="210" t="s">
         <v>1266</v>
       </c>
-      <c r="D1" s="211" t="s">
+      <c r="B1" s="211" t="s">
         <v>1267</v>
       </c>
-      <c r="E1" s="209" t="s">
+      <c r="C1" s="211" t="s">
         <v>1268</v>
+      </c>
+      <c r="D1" s="212" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E1" s="210" t="s">
+        <v>1270</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -26717,614 +26671,614 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B2" s="212" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C2" s="213">
-        <f>(SUM(Passif!D4:D15,Passif!D18:D19,Passif!D25:D26,Passif!D32:D33,Passif!D35:D36)-Actif!H30)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="214"/>
+        <v>1271</v>
+      </c>
+      <c r="B2" s="213" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C2" s="214">
+        <f>(SUM(Passif!D4:D15,Passif!D18:D19,Passif!D21:D22,Passif!D24:D25,Passif!D27:D28)-Actif!H30)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="215"/>
       <c r="E2" s="26" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B3" s="212" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C3" s="213" t="str">
-        <f>Actif!H49/Passif!D49</f>
+        <v>1271</v>
+      </c>
+      <c r="B3" s="213" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C3" s="214" t="str">
+        <f>Actif!H49/Passif!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D3" s="214"/>
+      <c r="D3" s="215"/>
       <c r="E3" s="26" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B4" s="215" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C4" s="213">
-        <f>(Actif!H31+SUM(Actif!H39))-Passif!D39</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="214"/>
+        <v>1271</v>
+      </c>
+      <c r="B4" s="216" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C4" s="214">
+        <f>(Actif!H31+SUM(Actif!H39))-Passif!D31</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="215"/>
       <c r="E4" s="26" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B5" s="212" t="s">
-        <v>1276</v>
-      </c>
-      <c r="C5" s="213" t="str">
+        <v>1271</v>
+      </c>
+      <c r="B5" s="213" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C5" s="214" t="str">
         <f>C2-C3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="216" t="s">
-        <v>1277</v>
+      <c r="D5" s="215"/>
+      <c r="E5" s="217" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B6" s="212" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C6" s="213">
+        <v>1271</v>
+      </c>
+      <c r="B6" s="213" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C6" s="214">
         <f>ESG!C20</f>
         <v>0</v>
       </c>
-      <c r="D6" s="214"/>
+      <c r="D6" s="215"/>
       <c r="E6" s="26" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B7" s="212" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C7" s="213" t="str">
+        <v>1271</v>
+      </c>
+      <c r="B7" s="213" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C7" s="214" t="str">
         <f>SUM(CPC!E4:E5)/Effectifs!D4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D7" s="214"/>
-      <c r="E7" s="217" t="s">
-        <v>1280</v>
+      <c r="D7" s="215"/>
+      <c r="E7" s="218" t="s">
+        <v>1282</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B8" s="212" t="s">
-        <v>1281</v>
-      </c>
-      <c r="C8" s="213">
+        <v>1271</v>
+      </c>
+      <c r="B8" s="213" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C8" s="214">
         <f>ESG!C43</f>
         <v>0</v>
       </c>
-      <c r="D8" s="214"/>
+      <c r="D8" s="215"/>
       <c r="E8" s="26"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B9" s="212" t="s">
-        <v>1283</v>
-      </c>
-      <c r="C9" s="214" t="str">
-        <f>Actif!H54/Passif!D49</f>
+        <v>1284</v>
+      </c>
+      <c r="B9" s="213" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C9" s="215" t="str">
+        <f>Actif!H54/Passif!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D9" s="214"/>
+      <c r="D9" s="215"/>
       <c r="E9" s="26" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B10" s="212" t="s">
         <v>1284</v>
       </c>
-      <c r="C10" s="214" t="str">
-        <f>(Actif!H54+Actif!H39+Actif!H31)/Passif!D49</f>
+      <c r="B10" s="213" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C10" s="215" t="str">
+        <f>(Actif!H54+Actif!H39+Actif!H31)/Passif!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D10" s="214"/>
+      <c r="D10" s="215"/>
       <c r="E10" s="26" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="26" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B11" s="212" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C11" s="214" t="str">
-        <f>(Actif!H54+Actif!H39)/Passif!D49</f>
+        <v>1284</v>
+      </c>
+      <c r="B11" s="213" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C11" s="215" t="str">
+        <f>(Actif!H54+Actif!H39)/Passif!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D11" s="214"/>
+      <c r="D11" s="215"/>
       <c r="E11" s="26" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="26" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B12" s="214" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C12" s="214" t="str">
+        <v>1284</v>
+      </c>
+      <c r="B12" s="215" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C12" s="215" t="str">
         <f>(ESG!C43-(C4-D4))/SUM(CPC!E4:E5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D12" s="214"/>
+      <c r="D12" s="215"/>
       <c r="E12" s="26"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B13" s="212" t="s">
-        <v>1290</v>
-      </c>
-      <c r="C13" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B13" s="213" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C13" s="215" t="str">
         <f>(Actif!H39*360)/(SUM(CPC!E4:E5)*1.2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D13" s="214"/>
-      <c r="E13" s="217" t="s">
-        <v>1291</v>
+      <c r="D13" s="215"/>
+      <c r="E13" s="218" t="s">
+        <v>1293</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B14" s="212" t="s">
-        <v>1292</v>
-      </c>
-      <c r="C14" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B14" s="213" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C14" s="215" t="str">
         <f>(CPC!E13)/ ((Actif!H32+Actif!I32)/2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D14" s="214"/>
+      <c r="D14" s="215"/>
       <c r="E14" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B15" s="212" t="s">
-        <v>1294</v>
-      </c>
-      <c r="C15" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B15" s="213" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C15" s="215" t="str">
         <f>360/C14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="214"/>
+      <c r="D15" s="215"/>
       <c r="E15" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B16" s="212" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C16" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B16" s="213" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C16" s="215" t="str">
         <f>CPC!E14/((Actif!H33+Actif!I33)/2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D16" s="214"/>
+      <c r="D16" s="215"/>
       <c r="E16" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B17" s="212" t="s">
-        <v>1296</v>
-      </c>
-      <c r="C17" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B17" s="213" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C17" s="215" t="str">
         <f>360/C16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="214"/>
+      <c r="D17" s="215"/>
       <c r="E17" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B18" s="212" t="s">
-        <v>1297</v>
-      </c>
-      <c r="C18" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B18" s="213" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C18" s="215" t="str">
         <f>(SUM(CPC!E5)*360)/ ((Actif!H36+Actif!I36)/2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D18" s="214"/>
+      <c r="D18" s="215"/>
       <c r="E18" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B19" s="212" t="s">
-        <v>1298</v>
-      </c>
-      <c r="C19" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B19" s="213" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C19" s="215" t="str">
         <f>360/C18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D19" s="214"/>
+      <c r="D19" s="215"/>
       <c r="E19" s="26" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B20" s="212" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C20" s="214" t="str">
-        <f>(Passif!D39*360)/(CPC!E14+CPC!E15)*1.2</f>
+        <v>1291</v>
+      </c>
+      <c r="B20" s="213" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C20" s="215" t="str">
+        <f>(Passif!D31*360)/(CPC!E14+CPC!E15)*1.2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D20" s="214"/>
-      <c r="E20" s="217" t="s">
-        <v>1300</v>
+      <c r="D20" s="215"/>
+      <c r="E20" s="218" t="s">
+        <v>1302</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B21" s="212" t="s">
-        <v>1301</v>
-      </c>
-      <c r="C21" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B21" s="213" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C21" s="215" t="str">
         <f>(SUM(CPC!E4:E5)*1.2)/SUM(Actif!H4,Actif!H13,Actif!H8)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D21" s="214"/>
+      <c r="D21" s="215"/>
       <c r="E21" s="26" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B22" s="212" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C22" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B22" s="213" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C22" s="215" t="str">
         <f>(SUM(CPC!E4:E5)*1.2)/Actif!H55</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D22" s="214"/>
+      <c r="D22" s="215"/>
       <c r="E22" s="26" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B23" s="212" t="s">
-        <v>1304</v>
-      </c>
-      <c r="C23" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B23" s="213" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C23" s="215" t="str">
         <f>(C13+C15+C17+C19) - C20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D23" s="214"/>
+      <c r="D23" s="215"/>
       <c r="E23" s="26"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B24" s="214" t="s">
-        <v>1305</v>
-      </c>
-      <c r="C24" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B24" s="215" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C24" s="215" t="str">
         <f>('Production '!C12-'Production '!D12)/'Production '!D12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D24" s="214"/>
-      <c r="E24" s="217" t="s">
-        <v>1306</v>
+      <c r="D24" s="215"/>
+      <c r="E24" s="218" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B25" s="214" t="s">
-        <v>1307</v>
-      </c>
-      <c r="C25" s="213" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B25" s="215" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C25" s="214" t="str">
         <f>SUM(CPC!G4:G5) - (SUM(CPC!H4:H5) )/ SUM(CPC!H4:H5)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="214"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D25" s="215"/>
       <c r="E25" s="26"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B26" s="218" t="s">
-        <v>1308</v>
-      </c>
-      <c r="C26" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B26" s="219" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C26" s="215" t="str">
         <f>(Actif!G4+Actif!G8+Actif!G13+Actif!G22)/(Actif!F4+Actif!F8+Actif!F13+Actif!F22)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D26" s="214"/>
+      <c r="D26" s="215"/>
       <c r="E26" s="26"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B27" s="214" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C27" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B27" s="215" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C27" s="215" t="str">
         <f>CPC!E17/SUM(CPC!E4:E6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="214"/>
+      <c r="D27" s="215"/>
       <c r="E27" s="26"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="26" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B28" s="214" t="s">
-        <v>1310</v>
-      </c>
-      <c r="C28" s="214" t="str">
+        <v>1291</v>
+      </c>
+      <c r="B28" s="215" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C28" s="215" t="str">
         <f>C4/SUM(CPC!E4:E5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="214"/>
+      <c r="D28" s="215"/>
       <c r="E28" s="26"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="217" t="s">
-        <v>1311</v>
-      </c>
-      <c r="B29" s="212" t="s">
-        <v>1312</v>
-      </c>
-      <c r="C29" s="214" t="str">
-        <f>Passif!D37/(Actif!H30+Ratios!C4)</f>
+      <c r="A29" s="218" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B29" s="213" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C29" s="215" t="str">
+        <f>Passif!D29/(Actif!H30+Ratios!C4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D29" s="214"/>
+      <c r="D29" s="215"/>
       <c r="E29" s="26"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="217" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B30" s="212" t="s">
-        <v>1314</v>
-      </c>
-      <c r="C30" s="214" t="str">
-        <f>Passif!D16/Passif!D37</f>
+      <c r="A30" s="218" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B30" s="213" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C30" s="215" t="str">
+        <f>Passif!D16/Passif!D29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D30" s="214"/>
+      <c r="D30" s="215"/>
       <c r="E30" s="26"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="26" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B31" s="212" t="s">
-        <v>1316</v>
-      </c>
-      <c r="C31" s="214" t="str">
-        <f>(Passif!D24+Passif!D38)/Passif!D16</f>
+        <v>1317</v>
+      </c>
+      <c r="B31" s="213" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C31" s="215" t="str">
+        <f>(Passif!D20+Passif!D30)/Passif!D16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D31" s="214"/>
+      <c r="D31" s="215"/>
       <c r="E31" s="26"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="26" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B32" s="212" t="s">
         <v>1317</v>
       </c>
-      <c r="C32" s="214" t="str">
-        <f>(Passif!D24-Ratios!C5)/Passif!D16</f>
+      <c r="B32" s="213" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C32" s="215" t="str">
+        <f>(Passif!D20-Ratios!C5)/Passif!D16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D32" s="214"/>
+      <c r="D32" s="215"/>
       <c r="E32" s="26"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="26" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B33" s="212" t="s">
-        <v>1318</v>
-      </c>
-      <c r="C33" s="214" t="str">
-        <f>Passif!D24/ESG!C43</f>
+        <v>1317</v>
+      </c>
+      <c r="B33" s="213" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C33" s="215" t="str">
+        <f>Passif!D20/ESG!C43</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D33" s="214"/>
+      <c r="D33" s="215"/>
       <c r="E33" s="26"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="26" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B34" s="214" t="s">
-        <v>1319</v>
-      </c>
-      <c r="C34" s="214" t="str">
-        <f>CPC!G33/(SUM(Passif!D25:D26)+Passif!D49)</f>
+        <v>1317</v>
+      </c>
+      <c r="B34" s="215" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C34" s="215" t="str">
+        <f>CPC!G33/(SUM(Passif!D21:D22)+Passif!D41)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D34" s="214"/>
+      <c r="D34" s="215"/>
       <c r="E34" s="26"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="26" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B35" s="214" t="s">
-        <v>1320</v>
-      </c>
-      <c r="C35" s="214" t="str">
+        <v>1317</v>
+      </c>
+      <c r="B35" s="215" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C35" s="215" t="str">
         <f>C6/CPC!E29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D35" s="214"/>
+      <c r="D35" s="215"/>
       <c r="E35" s="26"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B36" s="212" t="s">
-        <v>1322</v>
-      </c>
-      <c r="C36" s="214" t="str">
+        <v>1323</v>
+      </c>
+      <c r="B36" s="213" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C36" s="215" t="str">
         <f>C6/SUM(CPC!E4:E5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D36" s="214"/>
+      <c r="D36" s="215"/>
       <c r="E36" s="26"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B37" s="212" t="s">
         <v>1323</v>
       </c>
-      <c r="C37" s="214" t="str">
+      <c r="B37" s="213" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C37" s="215" t="str">
         <f>ESG!C8/ESG!C6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D37" s="214"/>
+      <c r="D37" s="215"/>
       <c r="E37" s="26"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B38" s="212" t="s">
-        <v>1324</v>
-      </c>
-      <c r="C38" s="214" t="str">
+        <v>1323</v>
+      </c>
+      <c r="B38" s="213" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C38" s="215" t="str">
         <f>CPC!E52/ SUM(CPC!E4:E5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D38" s="214"/>
+      <c r="D38" s="215"/>
       <c r="E38" s="26"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B39" s="212" t="s">
-        <v>1325</v>
-      </c>
-      <c r="C39" s="214" t="str">
+        <v>1323</v>
+      </c>
+      <c r="B39" s="213" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C39" s="215" t="str">
         <f>ESG!C30/ Actif!H30+Ratios!C4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D39" s="214"/>
+      <c r="D39" s="215"/>
       <c r="E39" s="26"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="26" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B40" s="212" t="s">
-        <v>1326</v>
-      </c>
-      <c r="C40" s="214" t="str">
+        <v>1323</v>
+      </c>
+      <c r="B40" s="213" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C40" s="215" t="str">
         <f>CPC!G55/Passif!D16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D40" s="214"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D40" s="215"/>
       <c r="E40" s="26"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="217" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B41" s="212" t="s">
-        <v>1328</v>
-      </c>
-      <c r="C41" s="214" t="str">
+      <c r="A41" s="218" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B41" s="213" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C41" s="215" t="str">
         <f>ESG!C44/Passif!D4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D41" s="214"/>
+      <c r="D41" s="215"/>
       <c r="E41" s="26"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="219" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B42" s="220" t="s">
+      <c r="A42" s="220" t="s">
         <v>1329</v>
       </c>
-      <c r="C42" s="220"/>
-      <c r="D42" s="212" t="s">
-        <v>1330</v>
+      <c r="B42" s="221" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C42" s="221"/>
+      <c r="D42" s="213" t="s">
+        <v>1332</v>
       </c>
       <c r="E42" s="26"/>
     </row>

</xml_diff>